<commit_message>
remove video edit， final requriement with houshidai
</commit_message>
<xml_diff>
--- a/youlin requirement.xlsx
+++ b/youlin requirement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zipai\Documents\GitHub\Youlin\digital product\publish\youlin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47B423C-DF49-4D8D-B55D-EDA3A683A663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE39FEEB-4644-4A65-9AD6-FAC7EF2F94EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,14 @@
     <sheet name="报价清单" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">报价清单!$B$2:$H$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">报价清单!$B$2:$H$37</definedName>
   </definedNames>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>北京逅时代功能报价清单</t>
   </si>
@@ -124,12 +125,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>Event 事件留言， 后台支持增减修改</t>
-  </si>
-  <si>
-    <t>小程序 Event/公约 数据库显示/编辑</t>
   </si>
   <si>
     <t>注册</t>
@@ -182,18 +177,6 @@
   </si>
   <si>
     <t>个人设置</t>
-  </si>
-  <si>
-    <t>优临微店</t>
-  </si>
-  <si>
-    <t>发现内容</t>
-  </si>
-  <si>
-    <t>速成游戏</t>
-  </si>
-  <si>
-    <t>家庭游戏</t>
   </si>
   <si>
     <t>费用合计</t>
@@ -223,15 +206,11 @@
 </t>
   </si>
   <si>
-    <t>微店</t>
+    <t>Event 事件留言</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>公众号-影片编辑</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>公众号-纪录片编辑</t>
+    <t>小程序 Event/公约</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -243,7 +222,7 @@
     <numFmt numFmtId="176" formatCode="&quot;¥ &quot;#,##0&quot; &quot;;&quot;(¥ &quot;#,##0\)"/>
     <numFmt numFmtId="177" formatCode="&quot;设计合计：¥&quot;#,##0;&quot;¥-&quot;#,##0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -359,23 +338,8 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="10"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,12 +376,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -868,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -927,9 +885,6 @@
     <xf numFmtId="49" fontId="10" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -981,126 +936,123 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="176" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="176" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1174,24 +1126,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="16" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2361,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFC42"/>
+  <dimension ref="A1:XFC38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="33.75" customHeight="1"/>
@@ -2389,9 +2323,9 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="26"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="27"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2406,144 +2340,144 @@
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
-      <c r="W1" s="43"/>
+      <c r="W1" s="41"/>
     </row>
     <row r="2" spans="1:23" ht="42.75" customHeight="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="44"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="42"/>
     </row>
     <row r="3" spans="1:23" ht="16.5" customHeight="1">
       <c r="A3" s="7"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="98" t="s">
+      <c r="C3" s="97"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="41"/>
-      <c r="W3" s="44"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="42"/>
     </row>
     <row r="4" spans="1:23" ht="16.5" customHeight="1">
       <c r="A4" s="7"/>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="98" t="s">
+      <c r="C4" s="97"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="44"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="42"/>
     </row>
     <row r="5" spans="1:23" ht="21" customHeight="1">
       <c r="A5" s="7"/>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="44"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="39"/>
+      <c r="W5" s="42"/>
     </row>
     <row r="6" spans="1:23" ht="33" customHeight="1">
       <c r="A6" s="8"/>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="44"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="42"/>
     </row>
     <row r="7" spans="1:23" ht="16.5" customHeight="1">
       <c r="A7" s="8"/>
@@ -2557,7 +2491,7 @@
       <c r="E7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -2566,104 +2500,104 @@
       <c r="H7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="41"/>
-      <c r="W7" s="44"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="42"/>
     </row>
     <row r="8" spans="1:23" ht="21.75" customHeight="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="60" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="82"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="44"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="42"/>
     </row>
     <row r="9" spans="1:23" ht="20.25" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="67"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="82"/>
-      <c r="F9" s="29"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="44"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="42"/>
     </row>
     <row r="10" spans="1:23" ht="21.75" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="68"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="29"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="41"/>
-      <c r="T10" s="41"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="41"/>
-      <c r="W10" s="44"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="39"/>
+      <c r="T10" s="39"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="39"/>
+      <c r="W10" s="42"/>
     </row>
     <row r="11" spans="1:23" ht="30" customHeight="1">
       <c r="A11" s="7"/>
@@ -2671,28 +2605,28 @@
         <v>17</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="23" t="s">
+      <c r="D11" s="79"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="41"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="41"/>
-      <c r="W11" s="44"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="39"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="39"/>
+      <c r="W11" s="42"/>
     </row>
     <row r="12" spans="1:23" ht="50" customHeight="1">
       <c r="A12" s="7"/>
@@ -2700,82 +2634,82 @@
         <v>19</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="81" t="s">
+      <c r="D12" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="82"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="44"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="42"/>
     </row>
     <row r="13" spans="1:23" ht="19.5" customHeight="1">
       <c r="A13" s="7"/>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="44"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="39"/>
+      <c r="W13" s="42"/>
     </row>
     <row r="14" spans="1:23" ht="27" customHeight="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="44"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="42"/>
     </row>
     <row r="15" spans="1:23" ht="20.25" customHeight="1">
       <c r="A15" s="7"/>
@@ -2789,808 +2723,690 @@
       <c r="E15" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="33"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="17" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="42"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="44"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="42"/>
     </row>
     <row r="16" spans="1:23" ht="37" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="66" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="46">
+      <c r="G16" s="22"/>
+      <c r="H16" s="74">
         <v>4000</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="41"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="41"/>
-      <c r="S16" s="41"/>
-      <c r="T16" s="41"/>
-      <c r="U16" s="41"/>
-      <c r="V16" s="41"/>
-      <c r="W16" s="44"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="42"/>
     </row>
     <row r="17" spans="1:23" ht="44" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="41"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="44"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="34"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="42"/>
     </row>
     <row r="18" spans="1:23" ht="41.5" customHeight="1">
       <c r="A18" s="7"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="41"/>
-      <c r="V18" s="41"/>
-      <c r="W18" s="44"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="34"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="39"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="39"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="39"/>
+      <c r="W18" s="42"/>
     </row>
     <row r="19" spans="1:23" ht="64.5" customHeight="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="35"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="32">
+        <v>31</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="34"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="31">
         <v>2500</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="41"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="41"/>
-      <c r="U19" s="41"/>
-      <c r="V19" s="41"/>
-      <c r="W19" s="44"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="39"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
+      <c r="W19" s="42"/>
     </row>
     <row r="20" spans="1:23" ht="57" customHeight="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="35"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="32">
+        <v>33</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="34"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="31">
         <v>2000</v>
       </c>
-      <c r="I20" s="42"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="41"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
-      <c r="U20" s="41"/>
-      <c r="V20" s="41"/>
-      <c r="W20" s="44"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
+      <c r="S20" s="39"/>
+      <c r="T20" s="39"/>
+      <c r="U20" s="39"/>
+      <c r="V20" s="39"/>
+      <c r="W20" s="42"/>
     </row>
     <row r="21" spans="1:23" ht="47" customHeight="1">
       <c r="A21" s="7"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="50"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="32">
+        <v>35</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="34"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="31">
         <v>2000</v>
       </c>
-      <c r="I21" s="42"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="41"/>
-      <c r="U21" s="41"/>
-      <c r="V21" s="41"/>
-      <c r="W21" s="44"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="39"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="39"/>
+      <c r="W21" s="42"/>
     </row>
     <row r="22" spans="1:23" ht="40" customHeight="1">
       <c r="A22" s="7"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="50"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="35"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="31">
+        <v>37</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="34"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="30">
         <v>3000</v>
       </c>
-      <c r="I22" s="42"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="41"/>
-      <c r="U22" s="41"/>
-      <c r="V22" s="41"/>
-      <c r="W22" s="44"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="39"/>
+      <c r="S22" s="39"/>
+      <c r="T22" s="39"/>
+      <c r="U22" s="39"/>
+      <c r="V22" s="39"/>
+      <c r="W22" s="42"/>
     </row>
     <row r="23" spans="1:23" ht="32" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="77">
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="75">
         <v>2000</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="41"/>
-      <c r="U23" s="41"/>
-      <c r="V23" s="41"/>
-      <c r="W23" s="44"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="42"/>
     </row>
     <row r="24" spans="1:23" ht="31" customHeight="1">
       <c r="A24" s="7"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="41"/>
-      <c r="T24" s="41"/>
-      <c r="U24" s="41"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="44"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="39"/>
+      <c r="S24" s="39"/>
+      <c r="T24" s="39"/>
+      <c r="U24" s="39"/>
+      <c r="V24" s="39"/>
+      <c r="W24" s="42"/>
     </row>
     <row r="25" spans="1:23" ht="31" customHeight="1">
       <c r="A25" s="7"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="41"/>
-      <c r="T25" s="41"/>
-      <c r="U25" s="41"/>
-      <c r="V25" s="41"/>
-      <c r="W25" s="44"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="39"/>
+      <c r="T25" s="39"/>
+      <c r="U25" s="39"/>
+      <c r="V25" s="39"/>
+      <c r="W25" s="42"/>
     </row>
     <row r="26" spans="1:23" ht="31" customHeight="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="36"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="108"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
-      <c r="T26" s="41"/>
-      <c r="U26" s="41"/>
-      <c r="V26" s="41"/>
-      <c r="W26" s="44"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="75">
+        <v>1000</v>
+      </c>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="39"/>
+      <c r="T26" s="39"/>
+      <c r="U26" s="39"/>
+      <c r="V26" s="39"/>
+      <c r="W26" s="42"/>
     </row>
     <row r="27" spans="1:23" ht="31" customHeight="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="73" t="s">
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="77">
-        <v>1000</v>
-      </c>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="41"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="41"/>
-      <c r="U27" s="41"/>
-      <c r="V27" s="41"/>
-      <c r="W27" s="44"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="39"/>
+      <c r="T27" s="39"/>
+      <c r="U27" s="39"/>
+      <c r="V27" s="39"/>
+      <c r="W27" s="42"/>
     </row>
     <row r="28" spans="1:23" ht="31" customHeight="1">
       <c r="A28" s="7"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="34" t="s">
+      <c r="B28" s="45"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="35"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
+      <c r="T28" s="39"/>
+      <c r="U28" s="39"/>
+      <c r="V28" s="39"/>
+      <c r="W28" s="42"/>
+    </row>
+    <row r="29" spans="1:23" ht="21.75" customHeight="1">
+      <c r="A29" s="7"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="53">
+        <f>H26+H23+H22+H21+H20+H19+H16</f>
+        <v>16500</v>
+      </c>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="39"/>
+      <c r="R29" s="39"/>
+      <c r="S29" s="39"/>
+      <c r="T29" s="39"/>
+      <c r="U29" s="39"/>
+      <c r="V29" s="39"/>
+      <c r="W29" s="42"/>
+    </row>
+    <row r="30" spans="1:23" ht="27" customHeight="1">
+      <c r="A30" s="7"/>
+      <c r="B30" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
-      <c r="S28" s="41"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="41"/>
-      <c r="V28" s="41"/>
-      <c r="W28" s="44"/>
-    </row>
-    <row r="29" spans="1:23" ht="31" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="34" t="s">
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="39"/>
+      <c r="R30" s="39"/>
+      <c r="S30" s="39"/>
+      <c r="T30" s="39"/>
+      <c r="U30" s="39"/>
+      <c r="V30" s="39"/>
+      <c r="W30" s="42"/>
+    </row>
+    <row r="31" spans="1:23" ht="16.5" customHeight="1">
+      <c r="A31" s="7"/>
+      <c r="B31" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="47"/>
+      <c r="E31" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="41"/>
-      <c r="V29" s="41"/>
-      <c r="W29" s="44"/>
-    </row>
-    <row r="30" spans="1:23" ht="31" customHeight="1">
-      <c r="A30" s="7"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="34" t="s">
+      <c r="F31" s="19"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="39"/>
+      <c r="R31" s="39"/>
+      <c r="S31" s="39"/>
+      <c r="T31" s="39"/>
+      <c r="U31" s="39"/>
+      <c r="V31" s="39"/>
+      <c r="W31" s="42"/>
+    </row>
+    <row r="32" spans="1:23" ht="16.5" customHeight="1">
+      <c r="A32" s="7"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="38">
-        <v>1000</v>
-      </c>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="41"/>
-      <c r="T30" s="41"/>
-      <c r="U30" s="41"/>
-      <c r="V30" s="41"/>
-      <c r="W30" s="44"/>
-    </row>
-    <row r="31" spans="1:23" ht="31" customHeight="1">
-      <c r="A31" s="7"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="73" t="s">
+      <c r="F32" s="19"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="39"/>
+      <c r="S32" s="39"/>
+      <c r="T32" s="39"/>
+      <c r="U32" s="39"/>
+      <c r="V32" s="39"/>
+      <c r="W32" s="42"/>
+    </row>
+    <row r="33" spans="1:23" ht="16.5" customHeight="1">
+      <c r="A33" s="7"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="39"/>
+      <c r="S33" s="39"/>
+      <c r="T33" s="39"/>
+      <c r="U33" s="39"/>
+      <c r="V33" s="39"/>
+      <c r="W33" s="42"/>
+    </row>
+    <row r="34" spans="1:23" ht="16.5" customHeight="1">
+      <c r="A34" s="7"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="106" t="s">
+      <c r="D34" s="50"/>
+      <c r="E34" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F31" s="103"/>
-      <c r="G31" s="104"/>
-      <c r="H31" s="107">
-        <v>1500</v>
-      </c>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="41"/>
-      <c r="P31" s="41"/>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="41"/>
-      <c r="U31" s="41"/>
-      <c r="V31" s="41"/>
-      <c r="W31" s="44"/>
-    </row>
-    <row r="32" spans="1:23" ht="31" customHeight="1">
-      <c r="A32" s="7"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="106" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="107"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="41"/>
-      <c r="O32" s="41"/>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="41"/>
-      <c r="S32" s="41"/>
-      <c r="T32" s="41"/>
-      <c r="U32" s="41"/>
-      <c r="V32" s="41"/>
-      <c r="W32" s="44"/>
-    </row>
-    <row r="33" spans="1:23" ht="21.75" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57">
-        <f>H30+H27+H31+H23+H22+H21+H20+H19+H16</f>
-        <v>19000</v>
-      </c>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41"/>
-      <c r="Q33" s="41"/>
-      <c r="R33" s="41"/>
-      <c r="S33" s="41"/>
-      <c r="T33" s="41"/>
-      <c r="U33" s="41"/>
-      <c r="V33" s="41"/>
-      <c r="W33" s="44"/>
-    </row>
-    <row r="34" spans="1:23" ht="27" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41"/>
-      <c r="M34" s="41"/>
-      <c r="N34" s="41"/>
-      <c r="O34" s="41"/>
-      <c r="P34" s="41"/>
-      <c r="Q34" s="41"/>
-      <c r="R34" s="41"/>
-      <c r="S34" s="41"/>
-      <c r="T34" s="41"/>
-      <c r="U34" s="41"/>
-      <c r="V34" s="41"/>
-      <c r="W34" s="44"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="39"/>
+      <c r="R34" s="39"/>
+      <c r="S34" s="39"/>
+      <c r="T34" s="39"/>
+      <c r="U34" s="39"/>
+      <c r="V34" s="39"/>
+      <c r="W34" s="42"/>
     </row>
     <row r="35" spans="1:23" ht="16.5" customHeight="1">
       <c r="A35" s="7"/>
-      <c r="B35" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" s="51" t="s">
-        <v>6</v>
-      </c>
+      <c r="B35" s="68"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="51"/>
       <c r="E35" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="19"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
+      <c r="O35" s="39"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="39"/>
+      <c r="R35" s="39"/>
+      <c r="S35" s="39"/>
+      <c r="T35" s="39"/>
+      <c r="U35" s="39"/>
+      <c r="V35" s="39"/>
+      <c r="W35" s="42"/>
+    </row>
+    <row r="36" spans="1:23" ht="37" customHeight="1">
+      <c r="A36" s="7"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" s="31"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
+      <c r="P36" s="39"/>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="39"/>
+      <c r="S36" s="39"/>
+      <c r="T36" s="39"/>
+      <c r="U36" s="39"/>
+      <c r="V36" s="39"/>
+      <c r="W36" s="42"/>
+    </row>
+    <row r="37" spans="1:23" ht="64" customHeight="1">
+      <c r="A37" s="7"/>
+      <c r="B37" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="41"/>
-      <c r="M35" s="41"/>
-      <c r="N35" s="41"/>
-      <c r="O35" s="41"/>
-      <c r="P35" s="41"/>
-      <c r="Q35" s="41"/>
-      <c r="R35" s="41"/>
-      <c r="S35" s="41"/>
-      <c r="T35" s="41"/>
-      <c r="U35" s="41"/>
-      <c r="V35" s="41"/>
-      <c r="W35" s="44"/>
-    </row>
-    <row r="36" spans="1:23" ht="16.5" customHeight="1">
-      <c r="A36" s="7"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="41"/>
-      <c r="S36" s="41"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="41"/>
-      <c r="V36" s="41"/>
-      <c r="W36" s="44"/>
-    </row>
-    <row r="37" spans="1:23" ht="16.5" customHeight="1">
-      <c r="A37" s="7"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="19"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="80"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="41"/>
-      <c r="O37" s="41"/>
-      <c r="P37" s="41"/>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="41"/>
-      <c r="S37" s="41"/>
-      <c r="T37" s="41"/>
-      <c r="U37" s="41"/>
-      <c r="V37" s="41"/>
-      <c r="W37" s="44"/>
-    </row>
-    <row r="38" spans="1:23" ht="16.5" customHeight="1">
-      <c r="A38" s="7"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="54"/>
-      <c r="E38" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="19"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="41"/>
-      <c r="V38" s="41"/>
-      <c r="W38" s="44"/>
-    </row>
-    <row r="39" spans="1:23" ht="16.5" customHeight="1">
-      <c r="A39" s="7"/>
-      <c r="B39" s="71"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F39" s="19"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="41"/>
-      <c r="M39" s="41"/>
-      <c r="N39" s="41"/>
-      <c r="O39" s="41"/>
-      <c r="P39" s="41"/>
-      <c r="Q39" s="41"/>
-      <c r="R39" s="41"/>
-      <c r="S39" s="41"/>
-      <c r="T39" s="41"/>
-      <c r="U39" s="41"/>
-      <c r="V39" s="41"/>
-      <c r="W39" s="44"/>
-    </row>
-    <row r="40" spans="1:23" ht="37" customHeight="1">
-      <c r="A40" s="7"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" s="32"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="41"/>
-      <c r="M40" s="41"/>
-      <c r="N40" s="41"/>
-      <c r="O40" s="41"/>
-      <c r="P40" s="41"/>
-      <c r="Q40" s="41"/>
-      <c r="R40" s="41"/>
-      <c r="S40" s="41"/>
-      <c r="T40" s="41"/>
-      <c r="U40" s="41"/>
-      <c r="V40" s="41"/>
-      <c r="W40" s="44"/>
-    </row>
-    <row r="41" spans="1:23" ht="64" customHeight="1">
-      <c r="A41" s="7"/>
-      <c r="B41" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="64"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="65"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="41"/>
-      <c r="M41" s="41"/>
-      <c r="N41" s="41"/>
-      <c r="O41" s="41"/>
-      <c r="P41" s="41"/>
-      <c r="Q41" s="41"/>
-      <c r="R41" s="41"/>
-      <c r="S41" s="41"/>
-      <c r="T41" s="41"/>
-      <c r="U41" s="41"/>
-      <c r="V41" s="41"/>
-      <c r="W41" s="44"/>
-    </row>
-    <row r="42" spans="1:23" ht="14" customHeight="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="41"/>
-      <c r="L42" s="41"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="41"/>
-      <c r="O42" s="41"/>
-      <c r="P42" s="41"/>
-      <c r="Q42" s="41"/>
-      <c r="R42" s="41"/>
-      <c r="S42" s="41"/>
-      <c r="T42" s="41"/>
-      <c r="U42" s="41"/>
-      <c r="V42" s="41"/>
-      <c r="W42" s="44"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
+      <c r="R37" s="39"/>
+      <c r="S37" s="39"/>
+      <c r="T37" s="39"/>
+      <c r="U37" s="39"/>
+      <c r="V37" s="39"/>
+      <c r="W37" s="42"/>
+    </row>
+    <row r="38" spans="1:23" ht="14" customHeight="1">
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="39"/>
+      <c r="Q38" s="39"/>
+      <c r="R38" s="39"/>
+      <c r="S38" s="39"/>
+      <c r="T38" s="39"/>
+      <c r="U38" s="39"/>
+      <c r="V38" s="39"/>
+      <c r="W38" s="42"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H41" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="35">
+  <autoFilter ref="B2:H37" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="33">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:H3"/>
@@ -3603,28 +3419,26 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B37:H37"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B31:B35"/>
     <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D26:D28"/>
     <mergeCell ref="H8:H12"/>
     <mergeCell ref="H16:H18"/>
     <mergeCell ref="H23:H25"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="H31:H33"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="B16:C32"/>
-    <mergeCell ref="C35:D37"/>
-    <mergeCell ref="C38:D39"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="B16:C28"/>
+    <mergeCell ref="C31:D33"/>
+    <mergeCell ref="C34:D35"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="B30:H30"/>
     <mergeCell ref="D16:D18"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -3633,7 +3447,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1 H7:H8 H15:H17 H23 H42 E33:H33 H35:H38 H40">
+  <conditionalFormatting sqref="H1 H7:H8 H15:H17 H23 H38 E29:H29 H31:H34 H36">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>